<commit_message>
4/11/25 Supply List Update
</commit_message>
<xml_diff>
--- a/Documentation/Buzzer Boards Supply List.xlsx
+++ b/Documentation/Buzzer Boards Supply List.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
   <si>
     <t>Buzzer Boards Supply List</t>
   </si>
@@ -37,7 +38,7 @@
     <t>walmart.com</t>
   </si>
   <si>
-    <t>Other microcontrollers will do. It just has to have __ data pins and be fast enough.</t>
+    <t>Must have 2 cores and enough data pins</t>
   </si>
   <si>
     <t>Buttons</t>
@@ -64,83 +65,101 @@
     <t>Any buzzer or speaker will do.</t>
   </si>
   <si>
-    <t>OLED Display</t>
-  </si>
-  <si>
-    <t>25ft. Ethernet Cable</t>
+    <t>3ft Ethernet Patch Cables</t>
+  </si>
+  <si>
+    <t>If you are willing to sacrifice the ability to plug/unplug buzzers, you could</t>
+  </si>
+  <si>
+    <t>Female Ethernet Plugs</t>
+  </si>
+  <si>
+    <t>5ft Ethernet cable for remote</t>
   </si>
   <si>
     <t>3D Printed Parts</t>
   </si>
   <si>
-    <t>If you don't have a printer, you can use stock boxes.</t>
+    <t>PLA</t>
   </si>
   <si>
     <t>Main Box</t>
   </si>
   <si>
+    <t>If you don't have a printer, you could buy stock boxes.</t>
+  </si>
+  <si>
+    <t>Remote Box</t>
+  </si>
+  <si>
     <t>Better yet, find a makerspace or friend that has a printer.</t>
   </si>
   <si>
-    <t>Control Box</t>
+    <t>Buzzer Boxes</t>
   </si>
   <si>
     <t>Most people would be glad to print a few parts in their spare time.</t>
   </si>
   <si>
-    <t>Buzzer Boxes</t>
-  </si>
-  <si>
     <t>Button Caps</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Wire</t>
-  </si>
-  <si>
-    <t>We assume builders will have ample supply of wire laying around. If not, start here.</t>
-  </si>
-  <si>
-    <t>Power Switch</t>
-  </si>
-  <si>
-    <t>If you want to bother. You might as well plug-unplug.</t>
-  </si>
-  <si>
-    <t>M3 Screws</t>
-  </si>
-  <si>
-    <t>These are nice if you have them, but otherwise, just use super glue.</t>
+    <t>Other Parts</t>
   </si>
   <si>
     <r>
-      <rPr/>
-      <t xml:space="preserve">You can go anywhere from </t>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <u/>
+      </rPr>
+      <t>Solid Core</t>
     </r>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> Wire</t>
+    </r>
+  </si>
+  <si>
+    <t>Heat Shrink Tubing</t>
+  </si>
+  <si>
+    <t>6m 60 IP30 WS2812B Lights</t>
+  </si>
+  <si>
+    <t>2ft Ethernet Patch Cables</t>
+  </si>
+  <si>
+    <t>5ft Ethernet cable for Control</t>
+  </si>
+  <si>
+    <t>Control Box</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
         <u/>
       </rPr>
-      <t>cheap buttons</t>
-    </r>
-    <r>
-      <rPr/>
-      <t xml:space="preserve"> to </t>
+      <t>Solid Core</t>
     </r>
     <r>
       <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Arial"/>
+        <color theme="1"/>
       </rPr>
-      <t>magnetic gaming keys</t>
+      <t xml:space="preserve"> Wire</t>
     </r>
-    <r>
-      <rPr/>
-      <t>.</t>
-    </r>
+  </si>
+  <si>
+    <t>Different Buttons</t>
   </si>
 </sst>
 </file>
@@ -170,13 +189,13 @@
       <color rgb="FF0000FF"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-    </font>
-    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="8">
@@ -212,14 +231,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB4A7D6"/>
-        <bgColor rgb="FFB4A7D6"/>
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCCC"/>
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
       </patternFill>
     </fill>
   </fills>
@@ -229,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -256,10 +275,10 @@
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -268,18 +287,9 @@
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -288,6 +298,16 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -297,6 +317,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -594,10 +618,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="6">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="C4" s="6">
-        <v>9.9</v>
+        <v>8.99</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>10</v>
@@ -614,7 +638,7 @@
         <v>1.0</v>
       </c>
       <c r="C5" s="6">
-        <v>5.48</v>
+        <v>6.15</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>13</v>
@@ -631,10 +655,10 @@
         <v>1.0</v>
       </c>
       <c r="C6" s="8">
-        <v>3.5</v>
+        <v>6.99</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -645,71 +669,83 @@
         <v>17</v>
       </c>
       <c r="B7" s="6">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="C7" s="8">
-        <v>6.99</v>
+        <v>13.43</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="E7" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="6">
-        <v>1.0</v>
+        <v>24.0</v>
       </c>
       <c r="C8" s="8">
-        <v>6.99</v>
+        <v>14.99</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11" t="s">
+      <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
+      <c r="B9" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4.99</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="B10" s="10">
+        <v>25.0</v>
+      </c>
+      <c r="C10" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
@@ -727,178 +763,142 @@
         <v>25</v>
       </c>
       <c r="B12" s="6">
-        <v>10.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="6">
-        <v>13.0</v>
+        <v>10.0</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="13">
-        <f t="shared" ref="B14:C14" si="1">SUM(B3:B13)</f>
-        <v>43</v>
-      </c>
-      <c r="C14" s="13">
-        <f t="shared" si="1"/>
-        <v>39.85</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
+      <c r="A14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="6">
+        <v>12.0</v>
+      </c>
+      <c r="E14" s="6"/>
     </row>
     <row r="15">
-      <c r="A15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="16"/>
-      <c r="X15" s="16"/>
-      <c r="Y15" s="16"/>
-      <c r="Z15" s="16"/>
+      <c r="A15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="13">
+        <f>SUM(B3:B14)</f>
+        <v>99</v>
+      </c>
+      <c r="C15" s="13">
+        <f>SUM(C3:C13)</f>
+        <v>67.53</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
     </row>
     <row r="16">
-      <c r="A16" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="17">
-        <v>1.0</v>
-      </c>
-      <c r="C16" s="18">
-        <v>11.99</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>29</v>
-      </c>
+      <c r="A16" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="20"/>
-      <c r="U16" s="20"/>
-      <c r="V16" s="20"/>
-      <c r="W16" s="20"/>
-      <c r="X16" s="20"/>
-      <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1.0</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B17" s="6"/>
       <c r="C17" s="8">
-        <v>4.17</v>
+        <v>15.19</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F17" s="6"/>
     </row>
     <row r="18">
-      <c r="A18" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="6">
-        <v>14.0</v>
-      </c>
-      <c r="C18" s="6">
-        <v>7.69</v>
+      <c r="A18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="8">
+        <v>6.17</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="22">
-        <v>13.0</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="23"/>
+      <c r="A19" s="18"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="22">
-      <c r="D22" s="22"/>
+      <c r="A22" s="20"/>
     </row>
     <row r="23">
-      <c r="D23" s="22"/>
-    </row>
-    <row r="25">
-      <c r="C25" s="8"/>
-      <c r="D25" s="22"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24">
+      <c r="D24" s="19"/>
+    </row>
+    <row r="26">
+      <c r="C26" s="8"/>
+      <c r="D26" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -911,11 +911,405 @@
     <hyperlink r:id="rId4" ref="D6"/>
     <hyperlink r:id="rId5" ref="D7"/>
     <hyperlink r:id="rId6" ref="D8"/>
-    <hyperlink r:id="rId7" ref="D16"/>
+    <hyperlink r:id="rId7" ref="D9"/>
     <hyperlink r:id="rId8" ref="D17"/>
     <hyperlink r:id="rId9" ref="D18"/>
-    <hyperlink r:id="rId10" ref="E19"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="26.13"/>
+    <col customWidth="1" min="2" max="2" width="7.63"/>
+    <col customWidth="1" min="3" max="3" width="7.13"/>
+    <col customWidth="1" min="5" max="5" width="61.88"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>56.0</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>24.72</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8">
+        <v>120.0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>17.98</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>6.99</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="6">
+        <v>100.0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>68.95</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6">
+        <v>250.0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>149.9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>34.77</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="22">
+        <v>250.0</v>
+      </c>
+      <c r="C10" s="22">
+        <v>50.0</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6">
+        <v>100.0</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="6">
+        <v>150.0</v>
+      </c>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="13">
+        <f>SUM(B3:B14)</f>
+        <v>1021</v>
+      </c>
+      <c r="C15" s="13">
+        <f>SUM(C3:C13)</f>
+        <v>409.31</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="8">
+        <v>15.19</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="8">
+        <v>6.17</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="8">
+        <v>120.0</v>
+      </c>
+      <c r="C19" s="6">
+        <v>39.6</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D3"/>
+    <hyperlink r:id="rId2" ref="D4"/>
+    <hyperlink r:id="rId3" ref="D5"/>
+    <hyperlink r:id="rId4" ref="D6"/>
+    <hyperlink r:id="rId5" ref="D7"/>
+    <hyperlink r:id="rId6" ref="D8"/>
+    <hyperlink r:id="rId7" ref="D9"/>
+    <hyperlink r:id="rId8" ref="D10"/>
+    <hyperlink r:id="rId9" ref="D17"/>
+    <hyperlink r:id="rId10" ref="D18"/>
+    <hyperlink r:id="rId11" ref="D19"/>
+  </hyperlinks>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>